<commit_message>
Add more patient metadata
</commit_message>
<xml_diff>
--- a/tables/additional_patient_metadata/patient_metadata_corrected.xlsx
+++ b/tables/additional_patient_metadata/patient_metadata_corrected.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="347">
   <si>
     <t xml:space="preserve">patient</t>
   </si>
@@ -634,9 +634,15 @@
     <t xml:space="preserve">Maier_Merad_2020_NSCLC_406</t>
   </si>
   <si>
+    <t xml:space="preserve">EGFR</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maier_Merad_2020_NSCLC_408</t>
   </si>
   <si>
+    <t xml:space="preserve">ERBB2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Maier_Merad_2020_NSCLC_410</t>
   </si>
   <si>
@@ -703,9 +709,6 @@
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH067</t>
   </si>
   <si>
-    <t xml:space="preserve">EGFR</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH103</t>
   </si>
   <si>
@@ -911,6 +914,9 @@
   </si>
   <si>
     <t xml:space="preserve">Wu_Zhou_2021_NSCLC_P1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">III or IV</t>
   </si>
   <si>
     <t xml:space="preserve">Wu_Zhou_2021_NSCLC_P10</t>
@@ -1061,8 +1067,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1138,13 +1145,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1166,11 +1185,11 @@
   </sheetPr>
   <dimension ref="A1:G304"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A246" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A183" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N210" activeCellId="0" sqref="N210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="50.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.63"/>
@@ -4008,243 +4027,657 @@
       <c r="A166" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="B166" s="0" t="n">
+        <v>69</v>
+      </c>
       <c r="C166" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D166" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E166" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F166" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G166" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="B167" s="0" t="n">
+        <v>79</v>
+      </c>
       <c r="C167" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D167" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E167" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F167" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G167" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="B168" s="0" t="n">
+        <v>77</v>
+      </c>
       <c r="C168" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
+      </c>
+      <c r="E168" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F168" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G168" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="B169" s="0" t="n">
+        <v>64</v>
+      </c>
       <c r="C169" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D169" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E169" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F169" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G169" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="B170" s="0" t="n">
+        <v>62</v>
+      </c>
       <c r="C170" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D170" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E170" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F170" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G170" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="B171" s="0" t="n">
+        <v>67</v>
+      </c>
       <c r="C171" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D171" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E171" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F171" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G171" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="B172" s="0" t="n">
+        <v>68</v>
+      </c>
       <c r="C172" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D172" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E172" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F172" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G172" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
+      </c>
+      <c r="B173" s="0" t="n">
+        <v>79</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D173" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="E173" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F173" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G173" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
+      </c>
+      <c r="B174" s="0" t="n">
+        <v>76</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D174" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E174" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F174" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G174" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
+      </c>
+      <c r="B175" s="0" t="n">
+        <v>66</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D175" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E175" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F175" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G175" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="B176" s="0" t="n">
+        <v>82</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
+      </c>
+      <c r="E176" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F176" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G176" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
+      </c>
+      <c r="B177" s="0" t="n">
+        <v>73</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D177" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E177" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F177" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G177" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="B178" s="0" t="n">
+        <v>57</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D178" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E178" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F178" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
+      </c>
+      <c r="B179" s="0" t="n">
+        <v>67</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D179" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E179" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F179" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G179" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
+      </c>
+      <c r="B180" s="0" t="n">
+        <v>61</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D180" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E180" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F180" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G180" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
+      </c>
+      <c r="B181" s="0" t="n">
+        <v>76</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D181" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="E181" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F181" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G181" s="0" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
+      </c>
+      <c r="B182" s="0" t="n">
+        <v>64</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D182" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E182" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F182" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G182" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
+      </c>
+      <c r="B183" s="0" t="n">
+        <v>64</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="E183" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F183" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G183" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
+      </c>
+      <c r="B184" s="0" t="n">
+        <v>71</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D184" s="0" t="s">
+        <v>187</v>
+      </c>
+      <c r="E184" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F184" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G184" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
+      </c>
+      <c r="B185" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D185" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E185" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F185" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G185" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
+      </c>
+      <c r="B186" s="0" t="n">
+        <v>72</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
+      </c>
+      <c r="E186" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F186" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G186" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
+      </c>
+      <c r="B187" s="0" t="n">
+        <v>75</v>
       </c>
       <c r="C187" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D187" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E187" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F187" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G187" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
+      </c>
+      <c r="B188" s="0" t="n">
+        <v>65</v>
       </c>
       <c r="C188" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D188" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="E188" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F188" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G188" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
+      </c>
+      <c r="B189" s="0" t="n">
+        <v>56</v>
       </c>
       <c r="C189" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="E189" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F189" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G189" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
+      </c>
+      <c r="B190" s="0" t="n">
+        <v>66</v>
       </c>
       <c r="C190" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D190" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E190" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F190" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G190" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
+      </c>
+      <c r="B191" s="0" t="n">
+        <v>73</v>
       </c>
       <c r="C191" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D191" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="E191" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F191" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G191" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
+      </c>
+      <c r="B192" s="0" t="n">
+        <v>74</v>
       </c>
       <c r="C192" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
+      </c>
+      <c r="E192" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F192" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G192" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
+      </c>
+      <c r="B193" s="0" t="n">
+        <v>76</v>
       </c>
       <c r="C193" s="0" t="s">
-        <v>60</v>
+        <v>74</v>
+      </c>
+      <c r="E193" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F193" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G193" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
+      </c>
+      <c r="B194" s="0" t="n">
+        <v>64</v>
       </c>
       <c r="C194" s="0" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="D194" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="E194" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F194" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G194" s="0" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
+      </c>
+      <c r="B195" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="C195" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E195" s="0" t="s">
         <v>83</v>
@@ -4258,13 +4691,16 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
+      </c>
+      <c r="B196" s="0" t="n">
+        <v>45</v>
       </c>
       <c r="C196" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E196" s="0" t="s">
         <v>83</v>
@@ -4278,13 +4714,16 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
+      </c>
+      <c r="B197" s="2" t="n">
+        <v>42</v>
       </c>
       <c r="C197" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E197" s="0" t="s">
         <v>83</v>
@@ -4298,13 +4737,16 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
+      </c>
+      <c r="B198" s="3" t="n">
+        <v>63</v>
       </c>
       <c r="C198" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E198" s="0" t="s">
         <v>83</v>
@@ -4318,13 +4760,16 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
+      </c>
+      <c r="B199" s="3" t="n">
+        <v>60</v>
       </c>
       <c r="C199" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E199" s="0" t="s">
         <v>83</v>
@@ -4338,13 +4783,16 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
+      </c>
+      <c r="B200" s="4" t="n">
+        <v>43</v>
       </c>
       <c r="C200" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E200" s="0" t="s">
         <v>75</v>
@@ -4358,13 +4806,16 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
+      </c>
+      <c r="B201" s="4" t="n">
+        <v>28</v>
       </c>
       <c r="C201" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E201" s="0" t="s">
         <v>83</v>
@@ -4378,13 +4829,16 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="B202" s="4" t="n">
+        <v>56</v>
       </c>
       <c r="C202" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E202" s="0" t="s">
         <v>83</v>
@@ -4398,13 +4852,16 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
+      </c>
+      <c r="B203" s="4" t="n">
+        <v>63</v>
       </c>
       <c r="C203" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E203" s="0" t="s">
         <v>83</v>
@@ -4418,13 +4875,16 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
+      </c>
+      <c r="B204" s="4" t="n">
+        <v>41</v>
       </c>
       <c r="C204" s="0" t="s">
         <v>74</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E204" s="0" t="s">
         <v>83</v>
@@ -4438,13 +4898,16 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
+      </c>
+      <c r="B205" s="4" t="n">
+        <v>62</v>
       </c>
       <c r="C205" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E205" s="0" t="s">
         <v>75</v>
@@ -4458,13 +4921,14 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>241</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="B206" s="3"/>
       <c r="C206" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E206" s="0" t="s">
         <v>75</v>
@@ -4478,13 +4942,16 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
+      </c>
+      <c r="B207" s="4" t="n">
+        <v>62</v>
       </c>
       <c r="C207" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E207" s="0" t="s">
         <v>83</v>
@@ -4498,13 +4965,16 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
+      </c>
+      <c r="B208" s="4" t="n">
+        <v>62</v>
       </c>
       <c r="C208" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D208" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E208" s="0" t="s">
         <v>83</v>
@@ -4518,13 +4988,16 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
+      </c>
+      <c r="B209" s="4" t="n">
+        <v>55</v>
       </c>
       <c r="C209" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E209" s="0" t="s">
         <v>83</v>
@@ -4538,13 +5011,14 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>246</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="B210" s="3"/>
       <c r="C210" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E210" s="0" t="s">
         <v>83</v>
@@ -4558,13 +5032,16 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
+      </c>
+      <c r="B211" s="4" t="n">
+        <v>53</v>
       </c>
       <c r="C211" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E211" s="0" t="s">
         <v>83</v>
@@ -4578,13 +5055,14 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>249</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="B212" s="3"/>
       <c r="C212" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E212" s="0" t="s">
         <v>83</v>
@@ -4598,13 +5076,16 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
+      </c>
+      <c r="B213" s="4" t="n">
+        <v>56</v>
       </c>
       <c r="C213" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E213" s="0" t="s">
         <v>83</v>
@@ -4618,13 +5099,16 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
+      </c>
+      <c r="B214" s="3" t="n">
+        <v>57</v>
       </c>
       <c r="C214" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E214" s="0" t="s">
         <v>83</v>
@@ -4633,18 +5117,21 @@
         <v>10</v>
       </c>
       <c r="G214" s="0" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
+      </c>
+      <c r="B215" s="4" t="n">
+        <v>59</v>
       </c>
       <c r="C215" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E215" s="0" t="s">
         <v>83</v>
@@ -4658,13 +5145,16 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
+      </c>
+      <c r="B216" s="3" t="n">
+        <v>71</v>
       </c>
       <c r="C216" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E216" s="0" t="s">
         <v>83</v>
@@ -4678,13 +5168,16 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
+      </c>
+      <c r="B217" s="4" t="n">
+        <v>58</v>
       </c>
       <c r="C217" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E217" s="0" t="s">
         <v>83</v>
@@ -4698,13 +5191,16 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="B218" s="4" t="n">
+        <v>54</v>
       </c>
       <c r="C218" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E218" s="0" t="s">
         <v>83</v>
@@ -4713,12 +5209,15 @@
         <v>12</v>
       </c>
       <c r="G218" s="0" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
+      </c>
+      <c r="B219" s="4" t="n">
+        <v>77</v>
       </c>
       <c r="C219" s="0" t="s">
         <v>81</v>
@@ -4738,13 +5237,16 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
+      </c>
+      <c r="B220" s="4" t="n">
+        <v>63</v>
       </c>
       <c r="C220" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E220" s="0" t="s">
         <v>75</v>
@@ -4758,13 +5260,16 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
+      </c>
+      <c r="B221" s="4" t="n">
+        <v>76</v>
       </c>
       <c r="C221" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E221" s="0" t="s">
         <v>83</v>
@@ -4778,13 +5283,16 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
+      </c>
+      <c r="B222" s="4" t="n">
+        <v>37</v>
       </c>
       <c r="C222" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E222" s="0" t="s">
         <v>83</v>
@@ -4798,13 +5306,16 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
+      </c>
+      <c r="B223" s="4" t="n">
+        <v>58</v>
       </c>
       <c r="C223" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E223" s="0" t="s">
         <v>83</v>
@@ -4818,13 +5329,16 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
+      </c>
+      <c r="B224" s="4" t="n">
+        <v>68</v>
       </c>
       <c r="C224" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E224" s="0" t="s">
         <v>75</v>
@@ -4838,13 +5352,16 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
+      </c>
+      <c r="B225" s="4" t="n">
+        <v>68</v>
       </c>
       <c r="C225" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E225" s="0" t="s">
         <v>75</v>
@@ -4858,13 +5375,16 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
+      </c>
+      <c r="B226" s="4" t="n">
+        <v>53</v>
       </c>
       <c r="C226" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="E226" s="0" t="s">
         <v>83</v>
@@ -4873,18 +5393,21 @@
         <v>12</v>
       </c>
       <c r="G226" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
+      </c>
+      <c r="B227" s="4" t="n">
+        <v>36</v>
       </c>
       <c r="C227" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D227" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E227" s="0" t="s">
         <v>83</v>
@@ -4898,7 +5421,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>8</v>
@@ -4906,7 +5429,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>8</v>
@@ -4914,7 +5437,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>8</v>
@@ -4922,7 +5445,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>8</v>
@@ -4930,7 +5453,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>8</v>
@@ -4938,7 +5461,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>8</v>
@@ -4946,7 +5469,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>8</v>
@@ -4954,7 +5477,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>8</v>
@@ -4962,7 +5485,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>8</v>
@@ -4970,7 +5493,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>8</v>
@@ -4978,7 +5501,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>63</v>
@@ -4995,7 +5518,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>55</v>
@@ -5012,7 +5535,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>26</v>
@@ -5029,7 +5552,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>57</v>
@@ -5046,7 +5569,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>49</v>
@@ -5063,7 +5586,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>22</v>
@@ -5080,7 +5603,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>47</v>
@@ -5097,7 +5620,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>21</v>
@@ -5114,7 +5637,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>75</v>
@@ -5131,7 +5654,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>64</v>
@@ -5148,7 +5671,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>51</v>
@@ -5165,7 +5688,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>65</v>
@@ -5185,7 +5708,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>70</v>
@@ -5205,7 +5728,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>64</v>
@@ -5225,7 +5748,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>62</v>
@@ -5242,7 +5765,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>58</v>
@@ -5259,7 +5782,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>58</v>
@@ -5276,7 +5799,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>69</v>
@@ -5293,7 +5816,10 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
+      </c>
+      <c r="B256" s="0" t="n">
+        <v>71</v>
       </c>
       <c r="C256" s="0" t="s">
         <v>74</v>
@@ -5301,10 +5827,16 @@
       <c r="F256" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="G256" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
+      </c>
+      <c r="B257" s="0" t="n">
+        <v>65</v>
       </c>
       <c r="C257" s="0" t="s">
         <v>74</v>
@@ -5312,10 +5844,16 @@
       <c r="F257" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G257" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>298</v>
+        <v>300</v>
+      </c>
+      <c r="B258" s="0" t="n">
+        <v>58</v>
       </c>
       <c r="C258" s="0" t="s">
         <v>60</v>
@@ -5323,32 +5861,50 @@
       <c r="F258" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="G258" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
+      </c>
+      <c r="B259" s="0" t="n">
+        <v>62</v>
       </c>
       <c r="C259" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F259" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="G259" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
+      </c>
+      <c r="B260" s="0" t="n">
+        <v>50</v>
       </c>
       <c r="C260" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F260" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="G260" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
+      </c>
+      <c r="B261" s="0" t="n">
+        <v>60</v>
       </c>
       <c r="C261" s="0" t="s">
         <v>74</v>
@@ -5356,10 +5912,16 @@
       <c r="F261" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G261" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
+      </c>
+      <c r="B262" s="0" t="n">
+        <v>64</v>
       </c>
       <c r="C262" s="0" t="s">
         <v>74</v>
@@ -5367,21 +5929,33 @@
       <c r="F262" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G262" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
+      </c>
+      <c r="B263" s="0" t="n">
+        <v>49</v>
       </c>
       <c r="C263" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F263" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G263" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
+      </c>
+      <c r="B264" s="0" t="n">
+        <v>71</v>
       </c>
       <c r="C264" s="0" t="s">
         <v>74</v>
@@ -5389,10 +5963,16 @@
       <c r="F264" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G264" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
+      </c>
+      <c r="B265" s="0" t="n">
+        <v>66</v>
       </c>
       <c r="C265" s="0" t="s">
         <v>74</v>
@@ -5400,10 +5980,16 @@
       <c r="F265" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G265" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
+      </c>
+      <c r="B266" s="0" t="n">
+        <v>55</v>
       </c>
       <c r="C266" s="0" t="s">
         <v>74</v>
@@ -5411,43 +5997,67 @@
       <c r="F266" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G266" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
+      </c>
+      <c r="B267" s="0" t="n">
+        <v>62</v>
       </c>
       <c r="C267" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F267" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G267" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
+      </c>
+      <c r="B268" s="0" t="n">
+        <v>59</v>
       </c>
       <c r="C268" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F268" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G268" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
+      </c>
+      <c r="B269" s="0" t="n">
+        <v>65</v>
       </c>
       <c r="C269" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F269" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G269" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
+      </c>
+      <c r="B270" s="0" t="n">
+        <v>67</v>
       </c>
       <c r="C270" s="0" t="s">
         <v>74</v>
@@ -5455,10 +6065,16 @@
       <c r="F270" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G270" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
+      </c>
+      <c r="B271" s="0" t="n">
+        <v>77</v>
       </c>
       <c r="C271" s="0" t="s">
         <v>74</v>
@@ -5466,21 +6082,33 @@
       <c r="F271" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G271" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
+      </c>
+      <c r="B272" s="0" t="n">
+        <v>52</v>
       </c>
       <c r="C272" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F272" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G272" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
+      </c>
+      <c r="B273" s="0" t="n">
+        <v>75</v>
       </c>
       <c r="C273" s="0" t="s">
         <v>74</v>
@@ -5488,10 +6116,16 @@
       <c r="F273" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G273" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
+      </c>
+      <c r="B274" s="0" t="n">
+        <v>53</v>
       </c>
       <c r="C274" s="0" t="s">
         <v>74</v>
@@ -5499,10 +6133,16 @@
       <c r="F274" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="G274" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
+      </c>
+      <c r="B275" s="0" t="n">
+        <v>68</v>
       </c>
       <c r="C275" s="0" t="s">
         <v>74</v>
@@ -5510,32 +6150,50 @@
       <c r="F275" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G275" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
+      </c>
+      <c r="B276" s="0" t="n">
+        <v>64</v>
       </c>
       <c r="C276" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F276" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="G276" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
+      </c>
+      <c r="B277" s="0" t="n">
+        <v>48</v>
       </c>
       <c r="C277" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F277" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G277" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
+      </c>
+      <c r="B278" s="0" t="n">
+        <v>67</v>
       </c>
       <c r="C278" s="0" t="s">
         <v>74</v>
@@ -5543,10 +6201,16 @@
       <c r="F278" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G278" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
+      </c>
+      <c r="B279" s="0" t="n">
+        <v>73</v>
       </c>
       <c r="C279" s="0" t="s">
         <v>74</v>
@@ -5554,10 +6218,16 @@
       <c r="F279" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G279" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
+      </c>
+      <c r="B280" s="0" t="n">
+        <v>53</v>
       </c>
       <c r="C280" s="0" t="s">
         <v>74</v>
@@ -5565,54 +6235,84 @@
       <c r="F280" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G280" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
+      </c>
+      <c r="B281" s="0" t="n">
+        <v>71</v>
       </c>
       <c r="C281" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F281" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="G281" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
+      </c>
+      <c r="B282" s="0" t="n">
+        <v>42</v>
       </c>
       <c r="C282" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F282" s="0" t="s">
         <v>12</v>
+      </c>
+      <c r="G282" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
+      </c>
+      <c r="B283" s="0" t="n">
+        <v>72</v>
       </c>
       <c r="C283" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F283" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G283" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
+      </c>
+      <c r="B284" s="0" t="n">
+        <v>63</v>
       </c>
       <c r="C284" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F284" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G284" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
+      </c>
+      <c r="B285" s="0" t="n">
+        <v>42</v>
       </c>
       <c r="C285" s="0" t="s">
         <v>74</v>
@@ -5620,10 +6320,16 @@
       <c r="F285" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G285" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
+      </c>
+      <c r="B286" s="0" t="n">
+        <v>73</v>
       </c>
       <c r="C286" s="0" t="s">
         <v>74</v>
@@ -5631,32 +6337,50 @@
       <c r="F286" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="G286" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
+      </c>
+      <c r="B287" s="0" t="n">
+        <v>55</v>
       </c>
       <c r="C287" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F287" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G287" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
+      </c>
+      <c r="B288" s="0" t="n">
+        <v>49</v>
       </c>
       <c r="C288" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F288" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G288" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
+      </c>
+      <c r="B289" s="0" t="n">
+        <v>58</v>
       </c>
       <c r="C289" s="0" t="s">
         <v>74</v>
@@ -5664,10 +6388,16 @@
       <c r="F289" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G289" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
+      </c>
+      <c r="B290" s="0" t="n">
+        <v>62</v>
       </c>
       <c r="C290" s="0" t="s">
         <v>74</v>
@@ -5675,10 +6405,16 @@
       <c r="F290" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G290" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
+      </c>
+      <c r="B291" s="0" t="n">
+        <v>60</v>
       </c>
       <c r="C291" s="0" t="s">
         <v>74</v>
@@ -5686,10 +6422,16 @@
       <c r="F291" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G291" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
+      </c>
+      <c r="B292" s="0" t="n">
+        <v>64</v>
       </c>
       <c r="C292" s="0" t="s">
         <v>60</v>
@@ -5697,21 +6439,33 @@
       <c r="F292" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G292" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
+      </c>
+      <c r="B293" s="0" t="n">
+        <v>62</v>
       </c>
       <c r="C293" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F293" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G293" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
+      </c>
+      <c r="B294" s="0" t="n">
+        <v>59</v>
       </c>
       <c r="C294" s="0" t="s">
         <v>74</v>
@@ -5719,10 +6473,16 @@
       <c r="F294" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G294" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
+      </c>
+      <c r="B295" s="0" t="n">
+        <v>71</v>
       </c>
       <c r="C295" s="0" t="s">
         <v>74</v>
@@ -5730,32 +6490,47 @@
       <c r="F295" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="G295" s="0" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
+      </c>
+      <c r="B296" s="0" t="n">
+        <v>35</v>
       </c>
       <c r="C296" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F296" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G296" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
+      </c>
+      <c r="B297" s="0" t="n">
+        <v>40</v>
       </c>
       <c r="C297" s="0" t="s">
         <v>81</v>
       </c>
       <c r="F297" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="G297" s="0" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B298" s="0" t="n">
         <v>79</v>
@@ -5772,7 +6547,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B299" s="0" t="n">
         <v>74</v>
@@ -5789,7 +6564,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B300" s="0" t="n">
         <v>61</v>
@@ -5806,7 +6581,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>83</v>
@@ -5823,7 +6598,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>72</v>
@@ -5840,7 +6615,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B303" s="0" t="n">
         <v>76</v>
@@ -5857,7 +6632,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B304" s="0" t="n">
         <v>63</v>

</xml_diff>

<commit_message>
unify tumor stages in annotation
</commit_message>
<xml_diff>
--- a/tables/additional_patient_metadata/patient_metadata_corrected.xlsx
+++ b/tables/additional_patient_metadata/patient_metadata_corrected.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="344">
   <si>
     <t xml:space="preserve">patient</t>
   </si>
@@ -781,9 +781,6 @@
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH217</t>
   </si>
   <si>
-    <t xml:space="preserve">IA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH218</t>
   </si>
   <si>
@@ -796,9 +793,6 @@
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH223</t>
   </si>
   <si>
-    <t xml:space="preserve">IIIA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH225</t>
   </si>
   <si>
@@ -821,9 +815,6 @@
   </si>
   <si>
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH248</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IIIB</t>
   </si>
   <si>
     <t xml:space="preserve">Maynard_Bivona_2020_NSCLC_TH266</t>
@@ -1145,17 +1136,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1185,11 +1172,11 @@
   </sheetPr>
   <dimension ref="A1:G304"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A183" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N210" activeCellId="0" sqref="N210"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A180" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G215" activeCellId="0" sqref="G215"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="50.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.63"/>
@@ -4739,7 +4726,7 @@
       <c r="A198" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="B198" s="3" t="n">
+      <c r="B198" s="2" t="n">
         <v>63</v>
       </c>
       <c r="C198" s="0" t="s">
@@ -4762,7 +4749,7 @@
       <c r="A199" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="B199" s="3" t="n">
+      <c r="B199" s="2" t="n">
         <v>60</v>
       </c>
       <c r="C199" s="0" t="s">
@@ -4785,7 +4772,7 @@
       <c r="A200" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B200" s="4" t="n">
+      <c r="B200" s="3" t="n">
         <v>43</v>
       </c>
       <c r="C200" s="0" t="s">
@@ -4808,7 +4795,7 @@
       <c r="A201" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B201" s="4" t="n">
+      <c r="B201" s="3" t="n">
         <v>28</v>
       </c>
       <c r="C201" s="0" t="s">
@@ -4831,7 +4818,7 @@
       <c r="A202" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="B202" s="4" t="n">
+      <c r="B202" s="3" t="n">
         <v>56</v>
       </c>
       <c r="C202" s="0" t="s">
@@ -4854,7 +4841,7 @@
       <c r="A203" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="B203" s="4" t="n">
+      <c r="B203" s="3" t="n">
         <v>63</v>
       </c>
       <c r="C203" s="0" t="s">
@@ -4877,7 +4864,7 @@
       <c r="A204" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B204" s="4" t="n">
+      <c r="B204" s="3" t="n">
         <v>41</v>
       </c>
       <c r="C204" s="0" t="s">
@@ -4900,7 +4887,7 @@
       <c r="A205" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="B205" s="4" t="n">
+      <c r="B205" s="3" t="n">
         <v>62</v>
       </c>
       <c r="C205" s="0" t="s">
@@ -4923,7 +4910,7 @@
       <c r="A206" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B206" s="3"/>
+      <c r="B206" s="2"/>
       <c r="C206" s="0" t="s">
         <v>81</v>
       </c>
@@ -4944,7 +4931,7 @@
       <c r="A207" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="B207" s="4" t="n">
+      <c r="B207" s="3" t="n">
         <v>62</v>
       </c>
       <c r="C207" s="0" t="s">
@@ -4967,7 +4954,7 @@
       <c r="A208" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B208" s="4" t="n">
+      <c r="B208" s="3" t="n">
         <v>62</v>
       </c>
       <c r="C208" s="0" t="s">
@@ -4990,7 +4977,7 @@
       <c r="A209" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B209" s="4" t="n">
+      <c r="B209" s="3" t="n">
         <v>55</v>
       </c>
       <c r="C209" s="0" t="s">
@@ -5013,7 +5000,7 @@
       <c r="A210" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B210" s="3"/>
+      <c r="B210" s="2"/>
       <c r="C210" s="0" t="s">
         <v>81</v>
       </c>
@@ -5034,7 +5021,7 @@
       <c r="A211" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B211" s="4" t="n">
+      <c r="B211" s="3" t="n">
         <v>53</v>
       </c>
       <c r="C211" s="0" t="s">
@@ -5057,7 +5044,7 @@
       <c r="A212" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B212" s="3"/>
+      <c r="B212" s="2"/>
       <c r="C212" s="0" t="s">
         <v>81</v>
       </c>
@@ -5078,7 +5065,7 @@
       <c r="A213" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B213" s="4" t="n">
+      <c r="B213" s="3" t="n">
         <v>56</v>
       </c>
       <c r="C213" s="0" t="s">
@@ -5101,7 +5088,7 @@
       <c r="A214" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B214" s="3" t="n">
+      <c r="B214" s="2" t="n">
         <v>57</v>
       </c>
       <c r="C214" s="0" t="s">
@@ -5117,14 +5104,14 @@
         <v>10</v>
       </c>
       <c r="G214" s="0" t="s">
-        <v>253</v>
+        <v>61</v>
       </c>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="B215" s="4" t="n">
+        <v>253</v>
+      </c>
+      <c r="B215" s="3" t="n">
         <v>59</v>
       </c>
       <c r="C215" s="0" t="s">
@@ -5145,9 +5132,9 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="B216" s="3" t="n">
+        <v>254</v>
+      </c>
+      <c r="B216" s="2" t="n">
         <v>71</v>
       </c>
       <c r="C216" s="0" t="s">
@@ -5168,9 +5155,9 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="B217" s="4" t="n">
+        <v>255</v>
+      </c>
+      <c r="B217" s="3" t="n">
         <v>58</v>
       </c>
       <c r="C217" s="0" t="s">
@@ -5191,9 +5178,9 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="B218" s="4" t="n">
+        <v>256</v>
+      </c>
+      <c r="B218" s="3" t="n">
         <v>54</v>
       </c>
       <c r="C218" s="0" t="s">
@@ -5209,14 +5196,14 @@
         <v>12</v>
       </c>
       <c r="G218" s="0" t="s">
-        <v>258</v>
+        <v>63</v>
       </c>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B219" s="4" t="n">
+        <v>257</v>
+      </c>
+      <c r="B219" s="3" t="n">
         <v>77</v>
       </c>
       <c r="C219" s="0" t="s">
@@ -5237,9 +5224,9 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B220" s="4" t="n">
+        <v>258</v>
+      </c>
+      <c r="B220" s="3" t="n">
         <v>63</v>
       </c>
       <c r="C220" s="0" t="s">
@@ -5260,9 +5247,9 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B221" s="4" t="n">
+        <v>259</v>
+      </c>
+      <c r="B221" s="3" t="n">
         <v>76</v>
       </c>
       <c r="C221" s="0" t="s">
@@ -5283,9 +5270,9 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="B222" s="4" t="n">
+        <v>260</v>
+      </c>
+      <c r="B222" s="3" t="n">
         <v>37</v>
       </c>
       <c r="C222" s="0" t="s">
@@ -5306,9 +5293,9 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="B223" s="4" t="n">
+        <v>261</v>
+      </c>
+      <c r="B223" s="3" t="n">
         <v>58</v>
       </c>
       <c r="C223" s="0" t="s">
@@ -5329,9 +5316,9 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B224" s="4" t="n">
+        <v>262</v>
+      </c>
+      <c r="B224" s="3" t="n">
         <v>68</v>
       </c>
       <c r="C224" s="0" t="s">
@@ -5352,9 +5339,9 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B225" s="4" t="n">
+        <v>263</v>
+      </c>
+      <c r="B225" s="3" t="n">
         <v>68</v>
       </c>
       <c r="C225" s="0" t="s">
@@ -5375,9 +5362,9 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="B226" s="4" t="n">
+        <v>264</v>
+      </c>
+      <c r="B226" s="3" t="n">
         <v>53</v>
       </c>
       <c r="C226" s="0" t="s">
@@ -5393,14 +5380,14 @@
         <v>12</v>
       </c>
       <c r="G226" s="0" t="s">
-        <v>267</v>
+        <v>63</v>
       </c>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B227" s="4" t="n">
+        <v>265</v>
+      </c>
+      <c r="B227" s="3" t="n">
         <v>36</v>
       </c>
       <c r="C227" s="0" t="s">
@@ -5421,7 +5408,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>8</v>
@@ -5429,7 +5416,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>8</v>
@@ -5437,7 +5424,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>8</v>
@@ -5445,7 +5432,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>8</v>
@@ -5453,7 +5440,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>8</v>
@@ -5461,7 +5448,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>8</v>
@@ -5469,7 +5456,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>8</v>
@@ -5477,7 +5464,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>8</v>
@@ -5485,7 +5472,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>8</v>
@@ -5493,7 +5480,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>8</v>
@@ -5501,7 +5488,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>63</v>
@@ -5518,7 +5505,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>55</v>
@@ -5535,7 +5522,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>26</v>
@@ -5552,7 +5539,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>57</v>
@@ -5569,7 +5556,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>49</v>
@@ -5586,7 +5573,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>22</v>
@@ -5603,7 +5590,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>47</v>
@@ -5620,7 +5607,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>21</v>
@@ -5637,7 +5624,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>75</v>
@@ -5654,7 +5641,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>64</v>
@@ -5671,7 +5658,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>51</v>
@@ -5688,7 +5675,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>65</v>
@@ -5708,7 +5695,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>70</v>
@@ -5728,7 +5715,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>64</v>
@@ -5748,7 +5735,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>62</v>
@@ -5765,7 +5752,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>58</v>
@@ -5782,7 +5769,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>58</v>
@@ -5799,7 +5786,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>69</v>
@@ -5816,7 +5803,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>71</v>
@@ -5828,12 +5815,12 @@
         <v>12</v>
       </c>
       <c r="G256" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>65</v>
@@ -5845,12 +5832,12 @@
         <v>10</v>
       </c>
       <c r="G257" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>58</v>
@@ -5862,12 +5849,12 @@
         <v>12</v>
       </c>
       <c r="G258" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>62</v>
@@ -5879,12 +5866,12 @@
         <v>12</v>
       </c>
       <c r="G259" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>50</v>
@@ -5896,12 +5883,12 @@
         <v>12</v>
       </c>
       <c r="G260" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>60</v>
@@ -5913,12 +5900,12 @@
         <v>10</v>
       </c>
       <c r="G261" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>64</v>
@@ -5930,12 +5917,12 @@
         <v>10</v>
       </c>
       <c r="G262" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>49</v>
@@ -5947,12 +5934,12 @@
         <v>10</v>
       </c>
       <c r="G263" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>71</v>
@@ -5964,12 +5951,12 @@
         <v>10</v>
       </c>
       <c r="G264" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>66</v>
@@ -5981,12 +5968,12 @@
         <v>10</v>
       </c>
       <c r="G265" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>55</v>
@@ -5998,12 +5985,12 @@
         <v>10</v>
       </c>
       <c r="G266" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>62</v>
@@ -6015,12 +6002,12 @@
         <v>10</v>
       </c>
       <c r="G267" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>59</v>
@@ -6032,12 +6019,12 @@
         <v>10</v>
       </c>
       <c r="G268" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>65</v>
@@ -6049,12 +6036,12 @@
         <v>10</v>
       </c>
       <c r="G269" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B270" s="0" t="n">
         <v>67</v>
@@ -6066,12 +6053,12 @@
         <v>10</v>
       </c>
       <c r="G270" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B271" s="0" t="n">
         <v>77</v>
@@ -6083,12 +6070,12 @@
         <v>10</v>
       </c>
       <c r="G271" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B272" s="0" t="n">
         <v>52</v>
@@ -6100,12 +6087,12 @@
         <v>10</v>
       </c>
       <c r="G272" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>75</v>
@@ -6117,12 +6104,12 @@
         <v>10</v>
       </c>
       <c r="G273" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>53</v>
@@ -6134,12 +6121,12 @@
         <v>12</v>
       </c>
       <c r="G274" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B275" s="0" t="n">
         <v>68</v>
@@ -6151,12 +6138,12 @@
         <v>10</v>
       </c>
       <c r="G275" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B276" s="0" t="n">
         <v>64</v>
@@ -6168,12 +6155,12 @@
         <v>12</v>
       </c>
       <c r="G276" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B277" s="0" t="n">
         <v>48</v>
@@ -6185,12 +6172,12 @@
         <v>10</v>
       </c>
       <c r="G277" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>67</v>
@@ -6202,12 +6189,12 @@
         <v>10</v>
       </c>
       <c r="G278" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>73</v>
@@ -6219,12 +6206,12 @@
         <v>10</v>
       </c>
       <c r="G279" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B280" s="0" t="n">
         <v>53</v>
@@ -6236,12 +6223,12 @@
         <v>10</v>
       </c>
       <c r="G280" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B281" s="0" t="n">
         <v>71</v>
@@ -6253,12 +6240,12 @@
         <v>12</v>
       </c>
       <c r="G281" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B282" s="0" t="n">
         <v>42</v>
@@ -6270,12 +6257,12 @@
         <v>12</v>
       </c>
       <c r="G282" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B283" s="0" t="n">
         <v>72</v>
@@ -6287,12 +6274,12 @@
         <v>10</v>
       </c>
       <c r="G283" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B284" s="0" t="n">
         <v>63</v>
@@ -6304,12 +6291,12 @@
         <v>10</v>
       </c>
       <c r="G284" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B285" s="0" t="n">
         <v>42</v>
@@ -6321,12 +6308,12 @@
         <v>10</v>
       </c>
       <c r="G285" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>73</v>
@@ -6338,12 +6325,12 @@
         <v>12</v>
       </c>
       <c r="G286" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>55</v>
@@ -6355,12 +6342,12 @@
         <v>10</v>
       </c>
       <c r="G287" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B288" s="0" t="n">
         <v>49</v>
@@ -6372,12 +6359,12 @@
         <v>10</v>
       </c>
       <c r="G288" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B289" s="0" t="n">
         <v>58</v>
@@ -6389,12 +6376,12 @@
         <v>10</v>
       </c>
       <c r="G289" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B290" s="0" t="n">
         <v>62</v>
@@ -6406,12 +6393,12 @@
         <v>10</v>
       </c>
       <c r="G290" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>60</v>
@@ -6423,12 +6410,12 @@
         <v>10</v>
       </c>
       <c r="G291" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>64</v>
@@ -6440,12 +6427,12 @@
         <v>10</v>
       </c>
       <c r="G292" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B293" s="0" t="n">
         <v>62</v>
@@ -6457,12 +6444,12 @@
         <v>10</v>
       </c>
       <c r="G293" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B294" s="0" t="n">
         <v>59</v>
@@ -6474,12 +6461,12 @@
         <v>10</v>
       </c>
       <c r="G294" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B295" s="0" t="n">
         <v>71</v>
@@ -6491,12 +6478,12 @@
         <v>10</v>
       </c>
       <c r="G295" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>35</v>
@@ -6508,12 +6495,12 @@
         <v>10</v>
       </c>
       <c r="G296" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>40</v>
@@ -6525,12 +6512,12 @@
         <v>10</v>
       </c>
       <c r="G297" s="0" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="B298" s="0" t="n">
         <v>79</v>
@@ -6547,7 +6534,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B299" s="0" t="n">
         <v>74</v>
@@ -6564,7 +6551,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="B300" s="0" t="n">
         <v>61</v>
@@ -6581,7 +6568,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>83</v>
@@ -6598,7 +6585,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>72</v>
@@ -6615,7 +6602,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B303" s="0" t="n">
         <v>76</v>
@@ -6632,7 +6619,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B304" s="0" t="n">
         <v>63</v>

</xml_diff>

<commit_message>
Make UMAP and cell-type marker plots
</commit_message>
<xml_diff>
--- a/tables/additional_patient_metadata/patient_metadata_corrected.xlsx
+++ b/tables/additional_patient_metadata/patient_metadata_corrected.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="345">
   <si>
     <t xml:space="preserve">patient</t>
   </si>
@@ -554,6 +554,9 @@
   </si>
   <si>
     <t xml:space="preserve">Laughney_Massague_2020_NSCLC_LX676</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
   </si>
   <si>
     <t xml:space="preserve">Laughney_Massague_2020_NSCLC_LX679</t>
@@ -1172,11 +1175,11 @@
   </sheetPr>
   <dimension ref="A1:G304"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A180" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G215" activeCellId="0" sqref="G215"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D152" activeCellId="0" sqref="D152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="50.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.63"/>
@@ -3788,6 +3791,9 @@
       <c r="C152" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="D152" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E152" s="0" t="s">
         <v>15</v>
       </c>
@@ -3797,13 +3803,13 @@
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C153" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D153" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E153" s="0" t="s">
         <v>15</v>
@@ -3814,13 +3820,13 @@
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C154" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D154" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E154" s="0" t="s">
         <v>15</v>
@@ -3831,10 +3837,13 @@
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C155" s="0" t="s">
         <v>81</v>
+      </c>
+      <c r="D155" s="0" t="s">
+        <v>178</v>
       </c>
       <c r="E155" s="0" t="s">
         <v>15</v>
@@ -3845,13 +3854,13 @@
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C156" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D156" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E156" s="0" t="s">
         <v>15</v>
@@ -3862,13 +3871,13 @@
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C157" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D157" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E157" s="0" t="s">
         <v>15</v>
@@ -3879,10 +3888,13 @@
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C158" s="0" t="s">
         <v>81</v>
+      </c>
+      <c r="D158" s="0" t="s">
+        <v>178</v>
       </c>
       <c r="E158" s="0" t="s">
         <v>9</v>
@@ -3893,13 +3905,13 @@
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C159" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D159" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E159" s="0" t="s">
         <v>15</v>
@@ -3910,13 +3922,13 @@
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C160" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D160" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E160" s="0" t="s">
         <v>83</v>
@@ -3927,7 +3939,7 @@
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>72</v>
@@ -3936,7 +3948,7 @@
         <v>8</v>
       </c>
       <c r="E161" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F161" s="0" t="s">
         <v>12</v>
@@ -3944,7 +3956,7 @@
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>43</v>
@@ -3961,7 +3973,7 @@
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>67</v>
@@ -3970,7 +3982,7 @@
         <v>8</v>
       </c>
       <c r="E163" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F163" s="0" t="s">
         <v>10</v>
@@ -3978,7 +3990,7 @@
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>57</v>
@@ -3987,7 +3999,7 @@
         <v>8</v>
       </c>
       <c r="E164" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F164" s="0" t="s">
         <v>10</v>
@@ -3995,7 +4007,7 @@
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>67</v>
@@ -4012,7 +4024,7 @@
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>69</v>
@@ -4021,7 +4033,7 @@
         <v>81</v>
       </c>
       <c r="D166" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E166" s="0" t="s">
         <v>83</v>
@@ -4035,7 +4047,7 @@
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>79</v>
@@ -4044,7 +4056,7 @@
         <v>81</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E167" s="0" t="s">
         <v>15</v>
@@ -4058,7 +4070,7 @@
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>77</v>
@@ -4066,6 +4078,9 @@
       <c r="C168" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="D168" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E168" s="0" t="s">
         <v>15</v>
       </c>
@@ -4078,7 +4093,7 @@
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>64</v>
@@ -4087,7 +4102,7 @@
         <v>81</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E169" s="0" t="s">
         <v>15</v>
@@ -4101,7 +4116,7 @@
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>62</v>
@@ -4110,7 +4125,7 @@
         <v>81</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E170" s="0" t="s">
         <v>15</v>
@@ -4124,7 +4139,7 @@
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>67</v>
@@ -4133,7 +4148,7 @@
         <v>81</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E171" s="0" t="s">
         <v>15</v>
@@ -4147,7 +4162,7 @@
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>68</v>
@@ -4156,7 +4171,7 @@
         <v>81</v>
       </c>
       <c r="D172" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E172" s="0" t="s">
         <v>9</v>
@@ -4170,7 +4185,7 @@
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>79</v>
@@ -4179,7 +4194,7 @@
         <v>81</v>
       </c>
       <c r="D173" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E173" s="0" t="s">
         <v>15</v>
@@ -4193,7 +4208,7 @@
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>76</v>
@@ -4202,7 +4217,7 @@
         <v>81</v>
       </c>
       <c r="D174" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E174" s="0" t="s">
         <v>15</v>
@@ -4216,7 +4231,7 @@
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="1" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>66</v>
@@ -4225,7 +4240,7 @@
         <v>81</v>
       </c>
       <c r="D175" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E175" s="0" t="s">
         <v>15</v>
@@ -4239,7 +4254,7 @@
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>82</v>
@@ -4247,6 +4262,9 @@
       <c r="C176" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="D176" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E176" s="0" t="s">
         <v>15</v>
       </c>
@@ -4259,7 +4277,7 @@
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="1" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>73</v>
@@ -4268,7 +4286,7 @@
         <v>81</v>
       </c>
       <c r="D177" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E177" s="0" t="s">
         <v>15</v>
@@ -4282,7 +4300,7 @@
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>57</v>
@@ -4291,7 +4309,7 @@
         <v>81</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E178" s="0" t="s">
         <v>15</v>
@@ -4302,7 +4320,7 @@
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>67</v>
@@ -4311,7 +4329,7 @@
         <v>81</v>
       </c>
       <c r="D179" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E179" s="0" t="s">
         <v>15</v>
@@ -4325,7 +4343,7 @@
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>61</v>
@@ -4348,7 +4366,7 @@
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B181" s="0" t="n">
         <v>76</v>
@@ -4371,7 +4389,7 @@
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B182" s="0" t="n">
         <v>64</v>
@@ -4380,7 +4398,7 @@
         <v>81</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E182" s="0" t="s">
         <v>9</v>
@@ -4394,7 +4412,7 @@
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B183" s="0" t="n">
         <v>64</v>
@@ -4402,6 +4420,9 @@
       <c r="C183" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="D183" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E183" s="0" t="s">
         <v>15</v>
       </c>
@@ -4414,7 +4435,7 @@
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B184" s="0" t="n">
         <v>71</v>
@@ -4423,7 +4444,7 @@
         <v>81</v>
       </c>
       <c r="D184" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E184" s="0" t="s">
         <v>15</v>
@@ -4437,7 +4458,7 @@
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B185" s="0" t="n">
         <v>68</v>
@@ -4446,7 +4467,7 @@
         <v>81</v>
       </c>
       <c r="D185" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E185" s="0" t="s">
         <v>9</v>
@@ -4460,7 +4481,7 @@
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B186" s="0" t="n">
         <v>72</v>
@@ -4468,6 +4489,9 @@
       <c r="C186" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="D186" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E186" s="0" t="s">
         <v>15</v>
       </c>
@@ -4480,7 +4504,7 @@
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B187" s="0" t="n">
         <v>75</v>
@@ -4489,7 +4513,7 @@
         <v>81</v>
       </c>
       <c r="D187" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E187" s="0" t="s">
         <v>15</v>
@@ -4503,7 +4527,7 @@
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B188" s="0" t="n">
         <v>65</v>
@@ -4512,7 +4536,7 @@
         <v>81</v>
       </c>
       <c r="D188" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E188" s="0" t="s">
         <v>15</v>
@@ -4526,7 +4550,7 @@
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B189" s="0" t="n">
         <v>56</v>
@@ -4534,6 +4558,9 @@
       <c r="C189" s="0" t="s">
         <v>81</v>
       </c>
+      <c r="D189" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E189" s="0" t="s">
         <v>9</v>
       </c>
@@ -4546,7 +4573,7 @@
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B190" s="0" t="n">
         <v>66</v>
@@ -4555,7 +4582,7 @@
         <v>81</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E190" s="0" t="s">
         <v>15</v>
@@ -4569,7 +4596,7 @@
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="1" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B191" s="0" t="n">
         <v>73</v>
@@ -4578,7 +4605,7 @@
         <v>81</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E191" s="0" t="s">
         <v>15</v>
@@ -4592,7 +4619,7 @@
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B192" s="0" t="n">
         <v>74</v>
@@ -4600,6 +4627,9 @@
       <c r="C192" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="D192" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E192" s="0" t="s">
         <v>15</v>
       </c>
@@ -4612,7 +4642,7 @@
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B193" s="0" t="n">
         <v>76</v>
@@ -4620,6 +4650,9 @@
       <c r="C193" s="0" t="s">
         <v>74</v>
       </c>
+      <c r="D193" s="0" t="s">
+        <v>178</v>
+      </c>
       <c r="E193" s="0" t="s">
         <v>15</v>
       </c>
@@ -4632,7 +4665,7 @@
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B194" s="0" t="n">
         <v>64</v>
@@ -4641,7 +4674,7 @@
         <v>81</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E194" s="0" t="s">
         <v>15</v>
@@ -4655,7 +4688,7 @@
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="1" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B195" s="0" t="n">
         <v>68</v>
@@ -4664,7 +4697,7 @@
         <v>81</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E195" s="0" t="s">
         <v>83</v>
@@ -4678,7 +4711,7 @@
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="1" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B196" s="0" t="n">
         <v>45</v>
@@ -4687,7 +4720,7 @@
         <v>81</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E196" s="0" t="s">
         <v>83</v>
@@ -4701,7 +4734,7 @@
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B197" s="2" t="n">
         <v>42</v>
@@ -4710,7 +4743,7 @@
         <v>81</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E197" s="0" t="s">
         <v>83</v>
@@ -4724,7 +4757,7 @@
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B198" s="2" t="n">
         <v>63</v>
@@ -4733,7 +4766,7 @@
         <v>81</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E198" s="0" t="s">
         <v>83</v>
@@ -4747,7 +4780,7 @@
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B199" s="2" t="n">
         <v>60</v>
@@ -4756,7 +4789,7 @@
         <v>81</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E199" s="0" t="s">
         <v>83</v>
@@ -4770,7 +4803,7 @@
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B200" s="3" t="n">
         <v>43</v>
@@ -4779,7 +4812,7 @@
         <v>81</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E200" s="0" t="s">
         <v>75</v>
@@ -4793,7 +4826,7 @@
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B201" s="3" t="n">
         <v>28</v>
@@ -4802,7 +4835,7 @@
         <v>81</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E201" s="0" t="s">
         <v>83</v>
@@ -4816,7 +4849,7 @@
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B202" s="3" t="n">
         <v>56</v>
@@ -4825,7 +4858,7 @@
         <v>81</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E202" s="0" t="s">
         <v>83</v>
@@ -4839,7 +4872,7 @@
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B203" s="3" t="n">
         <v>63</v>
@@ -4848,7 +4881,7 @@
         <v>81</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E203" s="0" t="s">
         <v>83</v>
@@ -4862,7 +4895,7 @@
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B204" s="3" t="n">
         <v>41</v>
@@ -4871,7 +4904,7 @@
         <v>74</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E204" s="0" t="s">
         <v>83</v>
@@ -4885,7 +4918,7 @@
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B205" s="3" t="n">
         <v>62</v>
@@ -4894,7 +4927,7 @@
         <v>81</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E205" s="0" t="s">
         <v>75</v>
@@ -4908,14 +4941,14 @@
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B206" s="2"/>
       <c r="C206" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E206" s="0" t="s">
         <v>75</v>
@@ -4929,7 +4962,7 @@
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B207" s="3" t="n">
         <v>62</v>
@@ -4938,7 +4971,7 @@
         <v>81</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E207" s="0" t="s">
         <v>83</v>
@@ -4952,7 +4985,7 @@
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B208" s="3" t="n">
         <v>62</v>
@@ -4961,7 +4994,7 @@
         <v>81</v>
       </c>
       <c r="D208" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E208" s="0" t="s">
         <v>83</v>
@@ -4975,7 +5008,7 @@
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B209" s="3" t="n">
         <v>55</v>
@@ -4984,7 +5017,7 @@
         <v>81</v>
       </c>
       <c r="D209" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E209" s="0" t="s">
         <v>83</v>
@@ -4998,14 +5031,14 @@
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B210" s="2"/>
       <c r="C210" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E210" s="0" t="s">
         <v>83</v>
@@ -5019,7 +5052,7 @@
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B211" s="3" t="n">
         <v>53</v>
@@ -5028,7 +5061,7 @@
         <v>81</v>
       </c>
       <c r="D211" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E211" s="0" t="s">
         <v>83</v>
@@ -5042,14 +5075,14 @@
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B212" s="2"/>
       <c r="C212" s="0" t="s">
         <v>81</v>
       </c>
       <c r="D212" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E212" s="0" t="s">
         <v>83</v>
@@ -5063,7 +5096,7 @@
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B213" s="3" t="n">
         <v>56</v>
@@ -5072,7 +5105,7 @@
         <v>81</v>
       </c>
       <c r="D213" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E213" s="0" t="s">
         <v>83</v>
@@ -5086,7 +5119,7 @@
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B214" s="2" t="n">
         <v>57</v>
@@ -5095,7 +5128,7 @@
         <v>81</v>
       </c>
       <c r="D214" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E214" s="0" t="s">
         <v>83</v>
@@ -5109,7 +5142,7 @@
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B215" s="3" t="n">
         <v>59</v>
@@ -5118,7 +5151,7 @@
         <v>81</v>
       </c>
       <c r="D215" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E215" s="0" t="s">
         <v>83</v>
@@ -5132,7 +5165,7 @@
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B216" s="2" t="n">
         <v>71</v>
@@ -5141,7 +5174,7 @@
         <v>81</v>
       </c>
       <c r="D216" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E216" s="0" t="s">
         <v>83</v>
@@ -5155,7 +5188,7 @@
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B217" s="3" t="n">
         <v>58</v>
@@ -5164,7 +5197,7 @@
         <v>81</v>
       </c>
       <c r="D217" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E217" s="0" t="s">
         <v>83</v>
@@ -5178,7 +5211,7 @@
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B218" s="3" t="n">
         <v>54</v>
@@ -5187,7 +5220,7 @@
         <v>81</v>
       </c>
       <c r="D218" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E218" s="0" t="s">
         <v>83</v>
@@ -5201,7 +5234,7 @@
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B219" s="3" t="n">
         <v>77</v>
@@ -5210,7 +5243,7 @@
         <v>81</v>
       </c>
       <c r="D219" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E219" s="0" t="s">
         <v>75</v>
@@ -5224,7 +5257,7 @@
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B220" s="3" t="n">
         <v>63</v>
@@ -5233,7 +5266,7 @@
         <v>81</v>
       </c>
       <c r="D220" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E220" s="0" t="s">
         <v>75</v>
@@ -5247,7 +5280,7 @@
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B221" s="3" t="n">
         <v>76</v>
@@ -5256,7 +5289,7 @@
         <v>81</v>
       </c>
       <c r="D221" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E221" s="0" t="s">
         <v>83</v>
@@ -5270,7 +5303,7 @@
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B222" s="3" t="n">
         <v>37</v>
@@ -5279,7 +5312,7 @@
         <v>81</v>
       </c>
       <c r="D222" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E222" s="0" t="s">
         <v>83</v>
@@ -5293,7 +5326,7 @@
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B223" s="3" t="n">
         <v>58</v>
@@ -5302,7 +5335,7 @@
         <v>81</v>
       </c>
       <c r="D223" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E223" s="0" t="s">
         <v>83</v>
@@ -5316,7 +5349,7 @@
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B224" s="3" t="n">
         <v>68</v>
@@ -5325,7 +5358,7 @@
         <v>81</v>
       </c>
       <c r="D224" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E224" s="0" t="s">
         <v>75</v>
@@ -5339,7 +5372,7 @@
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B225" s="3" t="n">
         <v>68</v>
@@ -5348,7 +5381,7 @@
         <v>81</v>
       </c>
       <c r="D225" s="0" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E225" s="0" t="s">
         <v>75</v>
@@ -5362,7 +5395,7 @@
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B226" s="3" t="n">
         <v>53</v>
@@ -5371,7 +5404,7 @@
         <v>81</v>
       </c>
       <c r="D226" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E226" s="0" t="s">
         <v>83</v>
@@ -5385,7 +5418,7 @@
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B227" s="3" t="n">
         <v>36</v>
@@ -5394,7 +5427,7 @@
         <v>81</v>
       </c>
       <c r="D227" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E227" s="0" t="s">
         <v>83</v>
@@ -5408,7 +5441,7 @@
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C228" s="0" t="s">
         <v>8</v>
@@ -5416,7 +5449,7 @@
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C229" s="0" t="s">
         <v>8</v>
@@ -5424,7 +5457,7 @@
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C230" s="0" t="s">
         <v>8</v>
@@ -5432,7 +5465,7 @@
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C231" s="0" t="s">
         <v>8</v>
@@ -5440,7 +5473,7 @@
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C232" s="0" t="s">
         <v>8</v>
@@ -5448,7 +5481,7 @@
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C233" s="0" t="s">
         <v>8</v>
@@ -5456,7 +5489,7 @@
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C234" s="0" t="s">
         <v>8</v>
@@ -5464,7 +5497,7 @@
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C235" s="0" t="s">
         <v>8</v>
@@ -5472,7 +5505,7 @@
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C236" s="0" t="s">
         <v>8</v>
@@ -5480,7 +5513,7 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C237" s="0" t="s">
         <v>8</v>
@@ -5488,7 +5521,7 @@
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B238" s="0" t="n">
         <v>63</v>
@@ -5505,7 +5538,7 @@
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B239" s="0" t="n">
         <v>55</v>
@@ -5522,7 +5555,7 @@
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B240" s="0" t="n">
         <v>26</v>
@@ -5539,7 +5572,7 @@
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B241" s="0" t="n">
         <v>57</v>
@@ -5556,7 +5589,7 @@
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B242" s="0" t="n">
         <v>49</v>
@@ -5573,7 +5606,7 @@
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="1" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B243" s="0" t="n">
         <v>22</v>
@@ -5590,7 +5623,7 @@
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B244" s="0" t="n">
         <v>47</v>
@@ -5607,7 +5640,7 @@
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B245" s="0" t="n">
         <v>21</v>
@@ -5624,7 +5657,7 @@
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="1" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B246" s="0" t="n">
         <v>75</v>
@@ -5641,7 +5674,7 @@
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B247" s="0" t="n">
         <v>64</v>
@@ -5658,7 +5691,7 @@
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B248" s="0" t="n">
         <v>51</v>
@@ -5675,7 +5708,7 @@
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="1" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B249" s="0" t="n">
         <v>65</v>
@@ -5695,7 +5728,7 @@
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A250" s="1" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B250" s="0" t="n">
         <v>70</v>
@@ -5715,7 +5748,7 @@
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A251" s="1" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B251" s="0" t="n">
         <v>64</v>
@@ -5735,7 +5768,7 @@
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="1" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B252" s="0" t="n">
         <v>62</v>
@@ -5752,7 +5785,7 @@
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A253" s="1" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B253" s="0" t="n">
         <v>58</v>
@@ -5769,7 +5802,7 @@
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A254" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B254" s="0" t="n">
         <v>58</v>
@@ -5786,7 +5819,7 @@
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A255" s="1" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B255" s="0" t="n">
         <v>69</v>
@@ -5803,7 +5836,7 @@
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="1" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B256" s="0" t="n">
         <v>71</v>
@@ -5815,12 +5848,12 @@
         <v>12</v>
       </c>
       <c r="G256" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A257" s="1" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B257" s="0" t="n">
         <v>65</v>
@@ -5832,12 +5865,12 @@
         <v>10</v>
       </c>
       <c r="G257" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A258" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="B258" s="0" t="n">
         <v>58</v>
@@ -5849,12 +5882,12 @@
         <v>12</v>
       </c>
       <c r="G258" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A259" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B259" s="0" t="n">
         <v>62</v>
@@ -5866,12 +5899,12 @@
         <v>12</v>
       </c>
       <c r="G259" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A260" s="1" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B260" s="0" t="n">
         <v>50</v>
@@ -5883,12 +5916,12 @@
         <v>12</v>
       </c>
       <c r="G260" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A261" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B261" s="0" t="n">
         <v>60</v>
@@ -5900,12 +5933,12 @@
         <v>10</v>
       </c>
       <c r="G261" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A262" s="1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B262" s="0" t="n">
         <v>64</v>
@@ -5917,12 +5950,12 @@
         <v>10</v>
       </c>
       <c r="G262" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A263" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B263" s="0" t="n">
         <v>49</v>
@@ -5934,12 +5967,12 @@
         <v>10</v>
       </c>
       <c r="G263" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A264" s="1" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B264" s="0" t="n">
         <v>71</v>
@@ -5951,12 +5984,12 @@
         <v>10</v>
       </c>
       <c r="G264" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A265" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B265" s="0" t="n">
         <v>66</v>
@@ -5968,12 +6001,12 @@
         <v>10</v>
       </c>
       <c r="G265" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A266" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B266" s="0" t="n">
         <v>55</v>
@@ -5985,12 +6018,12 @@
         <v>10</v>
       </c>
       <c r="G266" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A267" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B267" s="0" t="n">
         <v>62</v>
@@ -6002,12 +6035,12 @@
         <v>10</v>
       </c>
       <c r="G267" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A268" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B268" s="0" t="n">
         <v>59</v>
@@ -6019,12 +6052,12 @@
         <v>10</v>
       </c>
       <c r="G268" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A269" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B269" s="0" t="n">
         <v>65</v>
@@ -6036,12 +6069,12 @@
         <v>10</v>
       </c>
       <c r="G269" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A270" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B270" s="0" t="n">
         <v>67</v>
@@ -6053,12 +6086,12 @@
         <v>10</v>
       </c>
       <c r="G270" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A271" s="1" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B271" s="0" t="n">
         <v>77</v>
@@ -6070,12 +6103,12 @@
         <v>10</v>
       </c>
       <c r="G271" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A272" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B272" s="0" t="n">
         <v>52</v>
@@ -6087,12 +6120,12 @@
         <v>10</v>
       </c>
       <c r="G272" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A273" s="1" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B273" s="0" t="n">
         <v>75</v>
@@ -6104,12 +6137,12 @@
         <v>10</v>
       </c>
       <c r="G273" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A274" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B274" s="0" t="n">
         <v>53</v>
@@ -6121,12 +6154,12 @@
         <v>12</v>
       </c>
       <c r="G274" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A275" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B275" s="0" t="n">
         <v>68</v>
@@ -6138,12 +6171,12 @@
         <v>10</v>
       </c>
       <c r="G275" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A276" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B276" s="0" t="n">
         <v>64</v>
@@ -6155,12 +6188,12 @@
         <v>12</v>
       </c>
       <c r="G276" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A277" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B277" s="0" t="n">
         <v>48</v>
@@ -6172,12 +6205,12 @@
         <v>10</v>
       </c>
       <c r="G277" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A278" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B278" s="0" t="n">
         <v>67</v>
@@ -6189,12 +6222,12 @@
         <v>10</v>
       </c>
       <c r="G278" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A279" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B279" s="0" t="n">
         <v>73</v>
@@ -6206,12 +6239,12 @@
         <v>10</v>
       </c>
       <c r="G279" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A280" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B280" s="0" t="n">
         <v>53</v>
@@ -6223,12 +6256,12 @@
         <v>10</v>
       </c>
       <c r="G280" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A281" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B281" s="0" t="n">
         <v>71</v>
@@ -6240,12 +6273,12 @@
         <v>12</v>
       </c>
       <c r="G281" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A282" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B282" s="0" t="n">
         <v>42</v>
@@ -6257,12 +6290,12 @@
         <v>12</v>
       </c>
       <c r="G282" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A283" s="1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B283" s="0" t="n">
         <v>72</v>
@@ -6274,12 +6307,12 @@
         <v>10</v>
       </c>
       <c r="G283" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A284" s="1" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B284" s="0" t="n">
         <v>63</v>
@@ -6291,12 +6324,12 @@
         <v>10</v>
       </c>
       <c r="G284" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A285" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="B285" s="0" t="n">
         <v>42</v>
@@ -6308,12 +6341,12 @@
         <v>10</v>
       </c>
       <c r="G285" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A286" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B286" s="0" t="n">
         <v>73</v>
@@ -6325,12 +6358,12 @@
         <v>12</v>
       </c>
       <c r="G286" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A287" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B287" s="0" t="n">
         <v>55</v>
@@ -6342,12 +6375,12 @@
         <v>10</v>
       </c>
       <c r="G287" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A288" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B288" s="0" t="n">
         <v>49</v>
@@ -6359,12 +6392,12 @@
         <v>10</v>
       </c>
       <c r="G288" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B289" s="0" t="n">
         <v>58</v>
@@ -6376,12 +6409,12 @@
         <v>10</v>
       </c>
       <c r="G289" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A290" s="1" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B290" s="0" t="n">
         <v>62</v>
@@ -6393,12 +6426,12 @@
         <v>10</v>
       </c>
       <c r="G290" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A291" s="1" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B291" s="0" t="n">
         <v>60</v>
@@ -6410,12 +6443,12 @@
         <v>10</v>
       </c>
       <c r="G291" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A292" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B292" s="0" t="n">
         <v>64</v>
@@ -6427,12 +6460,12 @@
         <v>10</v>
       </c>
       <c r="G292" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A293" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="B293" s="0" t="n">
         <v>62</v>
@@ -6444,12 +6477,12 @@
         <v>10</v>
       </c>
       <c r="G293" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A294" s="1" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B294" s="0" t="n">
         <v>59</v>
@@ -6461,12 +6494,12 @@
         <v>10</v>
       </c>
       <c r="G294" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="1" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B295" s="0" t="n">
         <v>71</v>
@@ -6478,12 +6511,12 @@
         <v>10</v>
       </c>
       <c r="G295" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A296" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B296" s="0" t="n">
         <v>35</v>
@@ -6495,12 +6528,12 @@
         <v>10</v>
       </c>
       <c r="G296" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A297" s="1" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B297" s="0" t="n">
         <v>40</v>
@@ -6512,12 +6545,12 @@
         <v>10</v>
       </c>
       <c r="G297" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="1" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B298" s="0" t="n">
         <v>79</v>
@@ -6534,7 +6567,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A299" s="1" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B299" s="0" t="n">
         <v>74</v>
@@ -6551,7 +6584,7 @@
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A300" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="B300" s="0" t="n">
         <v>61</v>
@@ -6568,7 +6601,7 @@
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A301" s="1" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B301" s="0" t="n">
         <v>83</v>
@@ -6585,7 +6618,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A302" s="1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B302" s="0" t="n">
         <v>72</v>
@@ -6602,7 +6635,7 @@
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A303" s="1" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B303" s="0" t="n">
         <v>76</v>
@@ -6619,7 +6652,7 @@
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A304" s="1" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B304" s="0" t="n">
         <v>63</v>

</xml_diff>